<commit_message>
add case about query non-key but operation is get and cause issu
</commit_message>
<xml_diff>
--- a/src/test/resources/io.dingodb.test/testdata/cases/dql/casegroup3/sql_dql_cases3.xlsx
+++ b/src/test/resources/io.dingodb.test/testdata/cases/dql/casegroup3/sql_dql_cases3.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="47">
   <si>
     <t>TestID</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -119,44 +119,81 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>dqlc3_005</t>
+  </si>
+  <si>
+    <t>dqlc3_006</t>
+  </si>
+  <si>
+    <t>explain scan输出 - 主键int型</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>explain scan输出 - 主键varchar型</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>explain scan输出 - 主键date型</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>explain getByKey输出 - 主键int型</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>explain getByKey输出 - 主键varchar型</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>explain getByKey输出 - 主键date型</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Explain-scan</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Explain-key</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>dqlc3_007</t>
+  </si>
+  <si>
+    <t>dqlc3_008</t>
+  </si>
+  <si>
     <t>dqlc3_004</t>
-  </si>
-  <si>
-    <t>dqlc3_005</t>
-  </si>
-  <si>
-    <t>dqlc3_006</t>
-  </si>
-  <si>
-    <t>explain scan输出 - 主键int型</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>explain scan输出 - 主键varchar型</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>explain scan输出 - 主键date型</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>explain getByKey输出 - 主键int型</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>explain getByKey输出 - 主键varchar型</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>explain getByKey输出 - 主键date型</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Explain-scan</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Explain-key</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>select age from $schema17 where age=18</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>select name from $schema17 where name='zhangsan'</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>csv_containsAll</t>
+  </si>
+  <si>
+    <t>csv_containsAll</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>src/test/resources/io.dingodb.test/testdata/cases/dql/casegroup3/expectedresult/queryc3_007.csv</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>src/test/resources/io.dingodb.test/testdata/cases/dql/casegroup3/expectedresult/queryc3_008.csv</t>
+  </si>
+  <si>
+    <t>getByKey输出 - 非主键int型查询</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>getByKey输出 - 非主键varchar型查询</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -523,10 +560,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K7"/>
+  <dimension ref="A1:K9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -588,10 +625,10 @@
         <v>9</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>10</v>
@@ -614,10 +651,10 @@
         <v>9</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>19</v>
@@ -640,10 +677,10 @@
         <v>9</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F4" s="1" t="s">
         <v>23</v>
@@ -660,16 +697,16 @@
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A5" s="1" t="s">
-        <v>26</v>
+        <v>38</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>9</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F5" s="1" t="s">
         <v>10</v>
@@ -686,16 +723,16 @@
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A6" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>9</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F6" s="1" t="s">
         <v>19</v>
@@ -712,16 +749,16 @@
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A7" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>9</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F7" s="1" t="s">
         <v>23</v>
@@ -734,6 +771,64 @@
       </c>
       <c r="K7" s="1" t="s">
         <v>22</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A8" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="K8" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A9" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="J9" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="K9" s="1" t="s">
+        <v>41</v>
       </c>
     </row>
   </sheetData>

</xml_diff>